<commit_message>
Sentiment baselines were wrong because ru, tr and ja were included, also updated now
</commit_message>
<xml_diff>
--- a/results/baselines_sentiment.xlsx
+++ b/results/baselines_sentiment.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="14">
   <si>
     <t>Language</t>
   </si>
@@ -31,9 +31,6 @@
     <t>English</t>
   </si>
   <si>
-    <t>Russian</t>
-  </si>
-  <si>
     <t>Slovak</t>
   </si>
   <si>
@@ -55,13 +52,7 @@
     <t>Basque</t>
   </si>
   <si>
-    <t>Japanese</t>
-  </si>
-  <si>
     <t>Korean</t>
-  </si>
-  <si>
-    <t>Turkish</t>
   </si>
   <si>
     <t>Arabic</t>
@@ -425,7 +416,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -460,7 +451,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.671280276816609</v>
+        <v>0.8768796992481203</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -468,7 +459,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0.8768796992481203</v>
+        <v>0.7803203661327232</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -476,7 +467,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.7803203661327232</v>
+        <v>0.6045710139669871</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -484,7 +475,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0.6045710139669871</v>
+        <v>0.5138686131386861</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -492,7 +483,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0.5138686131386861</v>
+        <v>0.5921501706484642</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -500,7 +491,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0.5921501706484642</v>
+        <v>0.7455919395465995</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -508,7 +499,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>0.7455919395465995</v>
+        <v>0.8458149779735683</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -516,7 +507,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0.8458149779735683</v>
+        <v>0.58207343412527</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -524,7 +515,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>0.921</v>
+        <v>0.8325724493846764</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -532,31 +523,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>0.6840105232388191</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>0.5434782608695652</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15">
-        <v>0.8325724493846764</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16">
-        <v>0.9593450028232637</v>
+        <v>0.6817817014446228</v>
       </c>
     </row>
   </sheetData>
@@ -566,7 +533,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -601,7 +568,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.3356401384083045</v>
+        <v>0.4384398496240601</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -609,7 +576,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0.4384398496240601</v>
+        <v>0.3901601830663616</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -617,7 +584,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.3901601830663616</v>
+        <v>0.3022855069834935</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -625,7 +592,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0.3022855069834935</v>
+        <v>0.2569343065693431</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -633,7 +600,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0.2569343065693431</v>
+        <v>0.2960750853242321</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -641,7 +608,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0.2960750853242321</v>
+        <v>0.3727959697732998</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -649,7 +616,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>0.3727959697732998</v>
+        <v>0.4229074889867842</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -657,7 +624,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0.4229074889867842</v>
+        <v>0.291036717062635</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -665,7 +632,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>0.4605</v>
+        <v>0.4162862246923382</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -673,31 +640,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>0.3420052616194095</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>0.2717391304347826</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15">
-        <v>0.4162862246923382</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16">
-        <v>0.4796725014116319</v>
+        <v>0.3408908507223114</v>
       </c>
     </row>
   </sheetData>
@@ -707,7 +650,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -817,30 +760,6 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16">
-        <v>0.5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -848,7 +767,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -883,7 +802,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.4016563146997929</v>
+        <v>0.4672008012018027</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -891,7 +810,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0.4672008012018027</v>
+        <v>0.4383033419023136</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -899,7 +818,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.4383033419023136</v>
+        <v>0.3767804657472304</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -907,7 +826,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0.3767804657472304</v>
+        <v>0.3394406943105111</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -915,7 +834,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0.3394406943105111</v>
+        <v>0.3719185423365488</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -923,7 +842,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0.3719185423365488</v>
+        <v>0.4271284271284271</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -931,7 +850,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>0.4271284271284271</v>
+        <v>0.4582338902147972</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -939,7 +858,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0.4582338902147972</v>
+        <v>0.3679180887372014</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -947,7 +866,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>0.4794377928162415</v>
+        <v>0.4543189818575684</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -955,31 +874,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>0.4061794827286929</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>0.352112676056338</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15">
-        <v>0.4543189818575684</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16">
-        <v>0.4896253602305475</v>
+        <v>0.4053925077547125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>